<commit_message>
Add more cards for A1
</commit_message>
<xml_diff>
--- a/src/A1 Grammar Points.xlsx
+++ b/src/A1 Grammar Points.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonini/Projects/chinese_grammar_wiki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonini/Projects/chinese_grammar_wiki/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Simplified</t>
   </si>
@@ -207,13 +207,124 @@
   </si>
   <si>
     <t>you3</t>
+  </si>
+  <si>
+    <t>都</t>
+  </si>
+  <si>
+    <t>all / both / entirely / (used for emphasis) even / already / (not) at all</t>
+  </si>
+  <si>
+    <t>dou1</t>
+  </si>
+  <si>
+    <t>个</t>
+  </si>
+  <si>
+    <t>個</t>
+  </si>
+  <si>
+    <t>individual / this / that / size / classifier for people or objects in general</t>
+  </si>
+  <si>
+    <t>ge4</t>
+  </si>
+  <si>
+    <t>还是</t>
+  </si>
+  <si>
+    <t>還是</t>
+  </si>
+  <si>
+    <t>or / still / nevertheless</t>
+  </si>
+  <si>
+    <t>hai2 shi4</t>
+  </si>
+  <si>
+    <t>和</t>
+  </si>
+  <si>
+    <t>and / together with / with / sum / union / peace / harmony/ Taiwan pr. [han4] when it means "and" or "with"</t>
+  </si>
+  <si>
+    <t>he2</t>
+  </si>
+  <si>
+    <t>候</t>
+  </si>
+  <si>
+    <t>to wait / to inquire after / to watch / season / climate / (old) period of five days</t>
+  </si>
+  <si>
+    <t>hou4</t>
+  </si>
+  <si>
+    <t>时</t>
+  </si>
+  <si>
+    <t>時</t>
+  </si>
+  <si>
+    <t>o'clock / time / when / hour / season / period</t>
+  </si>
+  <si>
+    <t>shi2</t>
+  </si>
+  <si>
+    <t>岁</t>
+  </si>
+  <si>
+    <t>classifier for years (of age) / year / year (of crop harvests)</t>
+  </si>
+  <si>
+    <t>sui4</t>
+  </si>
+  <si>
+    <t>为</t>
+  </si>
+  <si>
+    <t>為</t>
+  </si>
+  <si>
+    <t>because of / for / to</t>
+  </si>
+  <si>
+    <t>wei4</t>
+  </si>
+  <si>
+    <t>也</t>
+  </si>
+  <si>
+    <t>also / too / (in Classical Chinese) final particle implying affirmation</t>
+  </si>
+  <si>
+    <t>ye3</t>
+  </si>
+  <si>
+    <t>在</t>
+  </si>
+  <si>
+    <t>(located) at / (to be) in / to exist / in the middle of doing sth / (indicating an action in progress)</t>
+  </si>
+  <si>
+    <t>zai4</t>
+  </si>
+  <si>
+    <t>怎</t>
+  </si>
+  <si>
+    <t>how</t>
+  </si>
+  <si>
+    <t>zen3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,12 +345,18 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
+      <sz val="21.6"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="17"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="21.6"/>
       <color rgb="FF2A3235"/>
       <name val="Times New Roman"/>
     </font>
@@ -275,10 +392,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -556,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -575,7 +690,7 @@
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -601,249 +716,546 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="139" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="47" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="47" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="47" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>